<commit_message>
Add calculation for population_density
</commit_message>
<xml_diff>
--- a/input/single_address.xlsx
+++ b/input/single_address.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\src\gis-toolkit\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52146D9-193D-4F12-9B0E-87AF09A63602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EAA004-BE74-4584-AD69-9E468B7F998E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -76,19 +76,19 @@
     <t>state</t>
   </si>
   <si>
-    <t>1745 T Street Southeast</t>
-  </si>
-  <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
     <t>zip</t>
   </si>
   <si>
     <t>street</t>
+  </si>
+  <si>
+    <t>560 Penstock Drive</t>
+  </si>
+  <si>
+    <t>Grass Valley</t>
+  </si>
+  <si>
+    <t>CA</t>
   </si>
 </sst>
 </file>
@@ -135,9 +135,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -430,7 +429,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,35 +437,35 @@
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="6">
-        <v>20020</v>
+      <c r="D2" s="5">
+        <v>95945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>